<commit_message>
105615 - FundingClaims Data Extract, Add Signed Column, template changes, tests
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.Operations.Reports.Reports/Templates/FundingClaimsDataExtractReport1920Template.xlsx
+++ b/src/ESFA.DC.Operations.Reports.Reports/Templates/FundingClaimsDataExtractReport1920Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSTS\DCT\DC-Operations-Reports\src\ESFA.DC.Operations.Reports.Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1662CBC8-C702-4673-AA2E-B5D857674F83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75EFBDF-9FCF-4852-BC75-2F2C95366D0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>SubmissionId</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>&amp;=FundingClaimDataExtractInfo.FundingClaimsDataExtract.CovidDeclaration</t>
+  </si>
+  <si>
+    <t>Signed</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaimDataExtractInfo.FundingClaimsDataExtract.Signed</t>
   </si>
 </sst>
 </file>
@@ -601,11 +607,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,20 +621,20 @@
     <col min="4" max="4" width="32" customWidth="1"/>
     <col min="5" max="5" width="17.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
-    <col min="11" max="11" width="39.140625" customWidth="1"/>
-    <col min="12" max="12" width="24.140625" customWidth="1"/>
-    <col min="13" max="13" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.140625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="20.140625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.42578125" customWidth="1"/>
+    <col min="7" max="8" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="12" max="12" width="39.140625" customWidth="1"/>
+    <col min="13" max="13" width="24.140625" customWidth="1"/>
+    <col min="14" max="14" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.140625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="20.140625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -648,40 +654,43 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -701,46 +710,49 @@
         <v>22</v>
       </c>
       <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" t="s">
         <v>33</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>25</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>26</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U266">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V266">
     <sortCondition ref="D2:D266"/>
     <sortCondition ref="C2:C266"/>
     <sortCondition ref="A2:A266"/>
-    <sortCondition ref="H2:H266"/>
-    <sortCondition ref="J2:J266"/>
+    <sortCondition ref="I2:I266"/>
+    <sortCondition ref="K2:K266"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
106066 - FundingClaimsExtract Report - report latest submission.
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.Operations.Reports.Reports/Templates/FundingClaimsDataExtractReport1920Template.xlsx
+++ b/src/ESFA.DC.Operations.Reports.Reports/Templates/FundingClaimsDataExtractReport1920Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\source\repos\DC-Operations-Reports\src\ESFA.DC.Operations.Reports.Reports\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSTS\DCT\DC-Operations-Reports\src\ESFA.DC.Operations.Reports.Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9CAF4D0-A558-4461-A92C-FAFE35B24602}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7865C0CD-DF0F-463D-A053-D0B202234DCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="377" windowWidth="18446" windowHeight="12677" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1920 Funding Claims Data" sheetId="1" r:id="rId1"/>
@@ -607,34 +607,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.84375" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="17.15234375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.84375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.84375" customWidth="1"/>
-    <col min="9" max="9" width="22.53515625" customWidth="1"/>
-    <col min="10" max="10" width="21.3828125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.53515625" customWidth="1"/>
-    <col min="12" max="12" width="39.15234375" customWidth="1"/>
-    <col min="13" max="13" width="24.15234375" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="12" max="12" width="39.140625" customWidth="1"/>
+    <col min="13" max="13" width="24.140625" customWidth="1"/>
     <col min="14" max="14" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.15234375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="20.15234375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="14.84375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.3828125" customWidth="1"/>
+    <col min="15" max="15" width="17.140625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="20.140625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -690,7 +690,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -744,11 +744,6 @@
       </c>
       <c r="R2" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="F4">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>